<commit_message>
changes in clinical acceptability files and code
</commit_message>
<xml_diff>
--- a/data_preparation/meta/auto_contours_review.xlsx
+++ b/data_preparation/meta/auto_contours_review.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="data_info" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="42">
   <si>
     <t xml:space="preserve">Curated Patient No</t>
   </si>
@@ -91,10 +91,46 @@
     <t xml:space="preserve">index</t>
   </si>
   <si>
-    <t xml:space="preserve">slice number</t>
+    <t xml:space="preserve">slice_no</t>
   </si>
   <si>
     <t xml:space="preserve">direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slice_coordinate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oar1_bowel_bag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oar1_bladder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oar1_hip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oar1_rectum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oar2_bowel_bag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oar2_bladder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oar2_hip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oar2_rectum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slice number</t>
   </si>
   <si>
     <t xml:space="preserve">slice coordinate</t>
@@ -116,18 +152,6 @@
   </si>
   <si>
     <t xml:space="preserve">rectum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">autocontour not excluding mesorectum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S</t>
   </si>
 </sst>
 </file>
@@ -191,16 +215,16 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
+      <left/>
       <right style="hair"/>
-      <top style="hair"/>
+      <top/>
       <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
+      <left style="hair"/>
       <right style="hair"/>
-      <top/>
+      <top style="hair"/>
       <bottom style="hair"/>
       <diagonal/>
     </border>
@@ -230,7 +254,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -251,24 +275,20 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -294,7 +314,7 @@
       <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.04"/>
@@ -493,13 +513,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="16.44"/>
@@ -507,7 +527,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -523,148 +543,164 @@
       <c r="E1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="F1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="I1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-    </row>
-    <row r="2" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="J1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="9" t="s">
+      <c r="K1" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="L1" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>81</v>
+        <v>71</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="H3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>71</v>
+        <v>61</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="J4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K4" s="1"/>
+      <c r="K4" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="L4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" s="3" t="n">
         <v>1</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="K5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="0" t="s">
-        <v>32</v>
+      <c r="L5" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>3</v>
@@ -679,37 +715,34 @@
         <v>1</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J6" s="1" t="n">
         <v>2</v>
       </c>
       <c r="K6" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L6" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="1" t="n">
         <v>31</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>41</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F7" s="1" t="n">
-        <v>2</v>
-      </c>
       <c r="G7" s="1" t="n">
         <v>1</v>
       </c>
@@ -717,37 +750,32 @@
         <v>1</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J7" s="1"/>
       <c r="K7" s="1" t="n">
         <v>2</v>
       </c>
       <c r="L7" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G8" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="H8" s="3" t="n">
         <v>1</v>
       </c>
@@ -755,25 +783,23 @@
         <v>2</v>
       </c>
       <c r="J8" s="1"/>
-      <c r="K8" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="K8" s="1"/>
       <c r="L8" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>3</v>
@@ -782,7 +808,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -792,16 +818,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>3</v>
@@ -810,7 +836,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -820,22 +846,22 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="n">
         <v>9</v>
-      </c>
-      <c r="B11" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H11" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11" s="1" t="n">
         <v>2</v>
@@ -843,30 +869,27 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="H12" s="3" t="n">
         <v>2</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -876,188 +899,200 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="L13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="I14" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I15" s="1"/>
+      <c r="I15" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="E16" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I16" s="1"/>
+      <c r="I16" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="E17" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I17" s="1"/>
+      <c r="I17" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="I18" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="E19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I19" s="1"/>
+      <c r="I19" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I20" s="1"/>
+      <c r="I20" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E21" s="1" t="n">
         <v>1</v>
@@ -1071,80 +1106,49 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="E22" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I22" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="E23" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1" t="n">
-        <v>132</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <v>129</v>
-      </c>
-      <c r="E24" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:L1"/>
-  </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E3:L24" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:L23" type="list">
       <formula1>"1,2,3,4"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1164,15 +1168,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -1188,67 +1192,79 @@
       <c r="E1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="F1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="I1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>29</v>
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="n">
         <v>1</v>
@@ -1256,22 +1272,24 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="H4" s="3" t="n">
         <v>1</v>
       </c>
@@ -1279,21 +1297,25 @@
       <c r="J4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
+      <c r="K4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="n">
@@ -1310,29 +1332,31 @@
         <v>1</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="3" t="n">
         <v>1</v>
@@ -1344,20 +1368,22 @@
       <c r="K6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="L6" s="1"/>
+      <c r="L6" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="n">
@@ -1376,27 +1402,29 @@
       <c r="K7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="L7" s="1"/>
+      <c r="L7" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" s="3" t="n">
         <v>1</v>
@@ -1408,54 +1436,56 @@
       <c r="K8" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="L8" s="1"/>
+      <c r="L8" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="E9" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="F9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="G9" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="G9" s="1"/>
       <c r="H9" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="J9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K9" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="K9" s="1"/>
       <c r="L9" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>2</v>
@@ -1480,26 +1510,26 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>2</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11" s="1" t="n">
         <v>2</v>
@@ -1508,52 +1538,52 @@
         <v>1</v>
       </c>
       <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="L11" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F12" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="J12" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="L12" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>2</v>
@@ -1574,25 +1604,23 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="3" t="n">
-        <v>1</v>
-      </c>
+      <c r="H14" s="3"/>
       <c r="I14" s="1" t="n">
         <v>2</v>
       </c>
@@ -1604,16 +1632,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>1</v>
@@ -1622,26 +1650,24 @@
       <c r="G15" s="1"/>
       <c r="H15" s="3"/>
       <c r="I15" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="L15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E16" s="1" t="n">
         <v>1</v>
@@ -1658,16 +1684,16 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E17" s="1" t="n">
         <v>1</v>
@@ -1684,16 +1710,16 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="E18" s="1" t="n">
         <v>1</v>
@@ -1710,16 +1736,16 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="E19" s="1" t="n">
         <v>1</v>
@@ -1736,16 +1762,16 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="E20" s="1" t="n">
         <v>1</v>
@@ -1762,19 +1788,19 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="E21" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1788,20 +1814,18 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>170</v>
-      </c>
-      <c r="E22" s="1" t="n">
-        <v>2</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="3"/>
@@ -1814,63 +1838,31 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="3"/>
       <c r="I23" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1" t="n">
-        <v>131</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <v>190</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:L1"/>
-  </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E3:L24" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:L23" type="list">
       <formula1>"1,2,3,4"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1890,15 +1882,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -1914,119 +1906,135 @@
       <c r="E1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="F1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="I1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="7" t="s">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="L3" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="H4" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="K4" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="L4" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="G5" s="1" t="n">
         <v>2</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="K5" s="1" t="n">
         <v>2</v>
       </c>
@@ -2036,20 +2044,20 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>2</v>
@@ -2059,7 +2067,7 @@
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>2</v>
@@ -2070,16 +2078,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="n">
@@ -2104,16 +2112,16 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="n">
@@ -2138,66 +2146,64 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="E9" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>3</v>
+      </c>
       <c r="F9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G9" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="G9" s="1"/>
       <c r="H9" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1" t="n">
+        <v>3</v>
+      </c>
       <c r="J9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K9" s="1" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="K9" s="1"/>
       <c r="L9" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="3" t="n">
-        <v>1</v>
-      </c>
+      <c r="H10" s="3"/>
       <c r="I10" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J10" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="n">
@@ -2206,51 +2212,45 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="3"/>
       <c r="I11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J11" s="1" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="L11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -2264,16 +2264,16 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>1</v>
@@ -2290,16 +2290,16 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>1</v>
@@ -2308,7 +2308,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="3"/>
       <c r="I14" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -2316,16 +2316,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>1</v>
@@ -2342,16 +2342,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E16" s="1" t="n">
         <v>1</v>
@@ -2360,7 +2360,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="3"/>
       <c r="I16" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -2368,16 +2368,16 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E17" s="1" t="n">
         <v>1</v>
@@ -2394,16 +2394,16 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E18" s="1" t="n">
         <v>1</v>
@@ -2420,19 +2420,19 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E19" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -2446,25 +2446,25 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="3"/>
       <c r="I20" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -2472,16 +2472,16 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="E21" s="1" t="n">
         <v>1</v>
@@ -2490,7 +2490,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="3"/>
       <c r="I21" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -2498,19 +2498,19 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="E22" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -2524,63 +2524,29 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>81</v>
-      </c>
-      <c r="E23" s="1" t="n">
-        <v>2</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <v>91</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:L1"/>
-  </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E3:L24" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:L23" type="list">
       <formula1>"1,2,3,4"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2600,15 +2566,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -2624,112 +2590,128 @@
       <c r="E1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="F1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="I1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="L3" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="H4" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K4" s="1"/>
+      <c r="K4" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="L4" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="n">
@@ -2754,16 +2736,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="n">
@@ -2773,7 +2755,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="n">
@@ -2788,16 +2770,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="n">
@@ -2807,68 +2789,68 @@
         <v>2</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K7" s="1" t="n">
         <v>2</v>
       </c>
       <c r="L7" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>3</v>
+      </c>
       <c r="F8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="G8" s="1"/>
       <c r="H8" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="I8" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>3</v>
+      </c>
       <c r="J8" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="K8" s="1" t="n">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K8" s="1"/>
       <c r="L8" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>1</v>
@@ -2890,29 +2872,29 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>2</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="3" t="n">
         <v>1</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J10" s="1" t="n">
         <v>1</v>
@@ -2924,80 +2906,72 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F11" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J11" s="1" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>2</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="3" t="n">
-        <v>3</v>
-      </c>
+      <c r="H12" s="3"/>
       <c r="I12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="L12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>2</v>
@@ -3006,7 +2980,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="3"/>
       <c r="I13" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -3014,16 +2988,16 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>2</v>
@@ -3032,7 +3006,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="3"/>
       <c r="I14" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -3040,16 +3014,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>2</v>
@@ -3058,7 +3032,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="3"/>
       <c r="I15" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -3066,16 +3040,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E16" s="1" t="n">
         <v>2</v>
@@ -3084,7 +3058,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="3"/>
       <c r="I16" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -3092,16 +3066,16 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E17" s="1" t="n">
         <v>2</v>
@@ -3110,7 +3084,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="3"/>
       <c r="I17" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -3118,25 +3092,25 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="E18" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="3"/>
       <c r="I18" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -3144,16 +3118,16 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="E19" s="1" t="n">
         <v>1</v>
@@ -3170,19 +3144,19 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -3196,20 +3170,18 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>94</v>
-      </c>
-      <c r="E21" s="1" t="n">
-        <v>3</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="3"/>
@@ -3222,16 +3194,16 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -3246,16 +3218,16 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -3268,41 +3240,9 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1" t="n">
-        <v>111</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <v>124</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:L1"/>
-  </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E3:L24" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:L23" type="list">
       <formula1>"1,2,3,4"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3324,66 +3264,66 @@
   </sheetPr>
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G36" activeCellId="0" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>29</v>
+      <c r="E2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3774,62 +3714,62 @@
       <selection pane="topLeft" activeCell="N13" activeCellId="0" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>29</v>
+      <c r="E2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>